<commit_message>
replaced SheetJS with XLSX-Populate, which is much better at preserving Excel formatting
</commit_message>
<xml_diff>
--- a/data/ADIDO Metadata Template.xlsx
+++ b/data/ADIDO Metadata Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\data-metadata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71803436-2F89-444F-89F7-98F37D641E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C0051E-675D-407F-86A4-0D1A50EA16ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10350" yWindow="5460" windowWidth="23320" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12650" yWindow="6450" windowWidth="23330" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Metadata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>** A note</t>
   </si>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -191,6 +191,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,21 +479,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5">
+        <v>3.1</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -497,12 +508,12 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -513,42 +524,221 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -557,10 +747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C95D46-1B5D-4F13-AA14-4F0E93E40CBC}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +762,7 @@
     <col min="5" max="5" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -589,7 +779,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -602,62 +792,309 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+    <row r="3" spans="1:12" s="8" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="G3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>